<commit_message>
Added 4 pin SIPP socket to parts list
Added 4 pin SIPP socket to the parts list for mounting of the Adafruit
DHT11 on a PCB.
</commit_message>
<xml_diff>
--- a/Hardware/WaterLeakAlarmPartsList.xlsx
+++ b/Hardware/WaterLeakAlarmPartsList.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>Item #</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>http://www.jameco.com/z/6100-14-R-Socket-IC-14-Pin-Machine-Tooled-Low-Profile-0-3-Inch-Wide_37197.html</t>
+  </si>
+  <si>
+    <t>4 pin SIPP socket</t>
+  </si>
+  <si>
+    <t>http://www.jameco.com/z/6100-1-4-Socket-SIPP-1x4-Pin-Machine-Tool-Pins-Soldertail-Female_164822.html</t>
+  </si>
+  <si>
+    <t>Best to mount the DHT11 in a socket.</t>
   </si>
 </sst>
 </file>
@@ -690,10 +699,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -771,7 +780,7 @@
     </row>
     <row r="4" spans="1:9" ht="45">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A25" si="0">A3+1</f>
+        <f t="shared" ref="A4:A26" si="0">A3+1</f>
         <v>2</v>
       </c>
       <c r="B4" s="2">
@@ -793,7 +802,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="10">
-        <f t="shared" ref="H4:H25" si="1">B4*G4</f>
+        <f t="shared" ref="H4:H26" si="1">B4*G4</f>
         <v>19</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1350,82 +1359,108 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="31.5" customHeight="1">
+    <row r="24" spans="1:9" ht="53.25" customHeight="1">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="4">
+        <v>164822</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0.59</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="1"/>
+        <v>0.59</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="31.5" customHeight="1">
+      <c r="A25" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G25" s="10">
         <v>1.37</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H25" s="10">
         <f t="shared" si="1"/>
         <v>2.74</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A25" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="2">
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A26" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D26" s="4">
         <v>452378</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G26" s="10">
         <v>2.79</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H26" s="10">
         <f t="shared" si="1"/>
         <v>2.79</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="F26" s="3"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-    </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="8" t="s">
-        <v>52</v>
-      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="12">
-        <f>SUM(H3:H26)</f>
-        <v>118.84</v>
-      </c>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:9">
+      <c r="A28" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="H28" s="12">
+        <f>SUM(H3:H27)</f>
+        <v>119.43</v>
+      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="F29" s="3"/>
@@ -1736,6 +1771,11 @@
       <c r="F90" s="3"/>
       <c r="G90" s="10"/>
       <c r="H90" s="10"/>
+    </row>
+    <row r="91" spans="6:8">
+      <c r="F91" s="3"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1756,11 +1796,11 @@
     <hyperlink ref="F15" r:id="rId15"/>
     <hyperlink ref="F7" r:id="rId16"/>
     <hyperlink ref="F8" r:id="rId17"/>
-    <hyperlink ref="F24" r:id="rId18"/>
+    <hyperlink ref="F25" r:id="rId18"/>
     <hyperlink ref="F6" r:id="rId19"/>
     <hyperlink ref="F14" r:id="rId20"/>
     <hyperlink ref="F21" r:id="rId21"/>
-    <hyperlink ref="F25" r:id="rId22"/>
+    <hyperlink ref="F26" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="59" orientation="landscape" r:id="rId23"/>

</xml_diff>